<commit_message>
data testid 46 osa
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Elise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB23E0F-92B8-4EE0-AD86-B6F7B37ECA7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8160641C-B9AC-49F9-98B5-04081CF5F1B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nädal 9" sheetId="11" r:id="rId1"/>
-    <sheet name="Nädal 8" sheetId="10" r:id="rId2"/>
-    <sheet name="Nädal 7" sheetId="9" r:id="rId3"/>
-    <sheet name="Nädal 6" sheetId="8" r:id="rId4"/>
-    <sheet name="Nädal 5" sheetId="7" r:id="rId5"/>
-    <sheet name="Nädal 4" sheetId="6" r:id="rId6"/>
-    <sheet name="Nädal 3" sheetId="5" r:id="rId7"/>
-    <sheet name="Nädal 2" sheetId="3" r:id="rId8"/>
-    <sheet name="Nädal 1" sheetId="1" r:id="rId9"/>
+    <sheet name="Nädal 10" sheetId="12" r:id="rId1"/>
+    <sheet name="Nädal 9" sheetId="11" r:id="rId2"/>
+    <sheet name="Nädal 8" sheetId="10" r:id="rId3"/>
+    <sheet name="Nädal 7" sheetId="9" r:id="rId4"/>
+    <sheet name="Nädal 6" sheetId="8" r:id="rId5"/>
+    <sheet name="Nädal 5" sheetId="7" r:id="rId6"/>
+    <sheet name="Nädal 4" sheetId="6" r:id="rId7"/>
+    <sheet name="Nädal 3" sheetId="5" r:id="rId8"/>
+    <sheet name="Nädal 2" sheetId="3" r:id="rId9"/>
+    <sheet name="Nädal 1" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="77">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -264,6 +265,12 @@
   </si>
   <si>
     <t>Andmebaasi error</t>
+  </si>
+  <si>
+    <t>45. osa</t>
+  </si>
+  <si>
+    <t>46 B osa</t>
   </si>
 </sst>
 </file>
@@ -1107,10 +1114,717 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1E625-AEC1-4959-BE11-B43C72FD971D}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="126" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="55">
+        <v>43905</v>
+      </c>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43920</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="55">
+        <v>43863</v>
+      </c>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="62"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <v>90</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <v>160</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>200</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <v>270</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>165</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43863</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>920</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E40E1A-5312-4ABD-B40E-50820F71C983}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="98" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B6" zoomScale="126" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1467,7 +2181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EA6F01-A62E-4B54-89CC-1CA4694260FA}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -1851,7 +2565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD152465-B78F-4330-B82E-1079DE07011D}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2166,7 +2880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D5B9A5-82EB-41D0-B31E-F472544F2A17}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2519,7 +3233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACF002-C02F-4F6D-A9DF-5CDFC75330FF}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2924,7 +3638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4BA9E6-34DD-4C1C-AEEF-5A72BA45E7B5}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -3309,7 +4023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8DD912-1C37-45A7-B4D1-E4B8ABC30324}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -3670,7 +4384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -4091,386 +4805,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="3.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="55">
-        <v>43863</v>
-      </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17">
-        <v>1</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21">
-        <v>90</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="22"/>
-      <c r="L7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0.84027777777777779</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.95138888888888884</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5">
-        <v>160</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5">
-        <v>200</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5">
-        <v>270</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5">
-        <v>165</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7">
-        <v>43863</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5">
-        <v>35</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>8</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
-        <v>9</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
-        <v>11</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="23">
-        <v>12</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="30">
-        <f>SUM(F7:F18)</f>
-        <v>920</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A2:J3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
testide errorid vähendatud, 5 tk alles
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453BFD4E-E7D8-4E86-B3BA-CBE5DDC45A5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7D48BA-AF20-4F8F-99E5-0313D4053D4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="510" windowWidth="14400" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>9. kodutöö</t>
+  </si>
+  <si>
+    <t>9. kodutöö + errorite eemaldamine</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1118,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="126" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1273,11 +1276,13 @@
       <c r="C9" s="8">
         <v>0.59722222222222221</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.68055555555555547</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1288,11 +1293,17 @@
         <v>4</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8">
+        <v>0.72222222222222221</v>
+      </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6">
+        <v>15</v>
+      </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>

</xml_diff>

<commit_message>
Mõned errorid eemaldatud, 51. osa tehtud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7D48BA-AF20-4F8F-99E5-0313D4053D4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB5B489-9005-49F1-8A99-03EC20C5A611}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="510" windowWidth="14400" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="190" windowWidth="14400" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 10" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>9. kodutöö + errorite eemaldamine</t>
+  </si>
+  <si>
+    <t>PluralSight kursus "KanBan Fundamentals"</t>
+  </si>
+  <si>
+    <t>9.kodutöö 51-51. osa</t>
+  </si>
+  <si>
+    <t>Errorite eemaldamine BaseRepository lehelt</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1E625-AEC1-4959-BE11-B43C72FD971D}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="126" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="126" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1238,7 +1247,9 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>40</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>75</v>
       </c>
@@ -1260,7 +1271,9 @@
       <c r="E8" s="39">
         <v>20</v>
       </c>
-      <c r="F8" s="40"/>
+      <c r="F8" s="40">
+        <v>236</v>
+      </c>
       <c r="G8" s="6" t="s">
         <v>75</v>
       </c>
@@ -1272,7 +1285,9 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="37">
+        <v>43921</v>
+      </c>
       <c r="C9" s="8">
         <v>0.59722222222222221</v>
       </c>
@@ -1280,7 +1295,9 @@
         <v>0.68055555555555547</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>120</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>76</v>
       </c>
@@ -1296,11 +1313,15 @@
       <c r="C10" s="8">
         <v>0.72222222222222221</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8">
+        <v>0.83680555555555547</v>
+      </c>
       <c r="E10" s="6">
         <v>15</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>150</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>76</v>
       </c>
@@ -1312,12 +1333,22 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="7">
+        <v>43922</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.78472222222222221</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="5">
+        <v>125</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="H11" s="31"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1326,12 +1357,22 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
+      <c r="B12" s="7">
+        <v>43923</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="E12" s="6">
+        <v>23</v>
+      </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -1341,11 +1382,15 @@
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -1430,7 +1475,7 @@
       <c r="E19" s="45"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>0</v>
+        <v>671</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
52. osa + ajalogi, 9. kodutöö tehtud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB5B489-9005-49F1-8A99-03EC20C5A611}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DE1CE7-8DAF-459A-8F03-BAEAD3E385EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="190" windowWidth="14400" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1110" windowWidth="14400" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 10" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="81">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -276,10 +276,13 @@
     <t>PluralSight kursus "KanBan Fundamentals"</t>
   </si>
   <si>
-    <t>9.kodutöö 51-51. osa</t>
-  </si>
-  <si>
-    <t>Errorite eemaldamine BaseRepository lehelt</t>
+    <t>9.kodutöö 51.osa</t>
+  </si>
+  <si>
+    <t>Errorite eemaldamine BaseRepository lehelt +52.osa</t>
+  </si>
+  <si>
+    <t>Clean Code fundamentals c# + konspekt</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1E625-AEC1-4959-BE11-B43C72FD971D}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="126" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="106" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1369,7 +1372,9 @@
       <c r="E12" s="6">
         <v>23</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>73</v>
+      </c>
       <c r="G12" s="8" t="s">
         <v>78</v>
       </c>
@@ -1385,9 +1390,13 @@
       <c r="C13" s="8">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>130</v>
+      </c>
       <c r="G13" s="6" t="s">
         <v>79</v>
       </c>
@@ -1400,11 +1409,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.80694444444444446</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="5">
+        <v>142</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1475,7 +1492,7 @@
       <c r="E19" s="45"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>671</v>
+        <v>1016</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1885,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E40E1A-5312-4ABD-B40E-50820F71C983}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" zoomScale="126" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="126" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
53. osa, q db context muudetud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DE1CE7-8DAF-459A-8F03-BAEAD3E385EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9634437-9944-45EE-8CDE-17B98250E9E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1110" windowWidth="14400" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nädal 10" sheetId="12" r:id="rId1"/>
-    <sheet name="Nädal 9" sheetId="11" r:id="rId2"/>
-    <sheet name="Nädal 8" sheetId="10" r:id="rId3"/>
-    <sheet name="Nädal 7" sheetId="9" r:id="rId4"/>
-    <sheet name="Nädal 6" sheetId="8" r:id="rId5"/>
-    <sheet name="Nädal 5" sheetId="7" r:id="rId6"/>
-    <sheet name="Nädal 4" sheetId="6" r:id="rId7"/>
-    <sheet name="Nädal 3" sheetId="5" r:id="rId8"/>
-    <sheet name="Nädal 2" sheetId="3" r:id="rId9"/>
-    <sheet name="Nädal 1" sheetId="1" r:id="rId10"/>
+    <sheet name="Nädal 11" sheetId="13" r:id="rId1"/>
+    <sheet name="Nädal 10" sheetId="12" r:id="rId2"/>
+    <sheet name="Nädal 9" sheetId="11" r:id="rId3"/>
+    <sheet name="Nädal 8" sheetId="10" r:id="rId4"/>
+    <sheet name="Nädal 7" sheetId="9" r:id="rId5"/>
+    <sheet name="Nädal 6" sheetId="8" r:id="rId6"/>
+    <sheet name="Nädal 5" sheetId="7" r:id="rId7"/>
+    <sheet name="Nädal 4" sheetId="6" r:id="rId8"/>
+    <sheet name="Nädal 3" sheetId="5" r:id="rId9"/>
+    <sheet name="Nädal 2" sheetId="3" r:id="rId10"/>
+    <sheet name="Nädal 1" sheetId="1" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="85">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -283,6 +284,18 @@
   </si>
   <si>
     <t>Clean Code fundamentals c# + konspekt</t>
+  </si>
+  <si>
+    <t>Kordamine kontrolltööks MVC vs Razor Pages</t>
+  </si>
+  <si>
+    <t>Viimane kordamine tööks</t>
+  </si>
+  <si>
+    <t>6-12aprill</t>
+  </si>
+  <si>
+    <t>10. kodutöö</t>
   </si>
 </sst>
 </file>
@@ -685,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -813,6 +826,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,11 +1149,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1E625-AEC1-4959-BE11-B43C72FD971D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BEF23C-5D4F-4A0C-A005-79341DDADDA7}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="106" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1187,12 +1210,12 @@
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
-        <v>43905</v>
-      </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="G4" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="57"/>
@@ -1241,20 +1264,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="7">
-        <v>43920</v>
+        <v>43927</v>
       </c>
       <c r="C7" s="8">
-        <v>0.73611111111111116</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.76388888888888884</v>
-      </c>
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="5">
-        <v>40</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="6" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="20"/>
@@ -1265,22 +1284,11 @@
         <v>2</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="38">
-        <v>0.78472222222222221</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.94861111111111107</v>
-      </c>
-      <c r="E8" s="39">
-        <v>20</v>
-      </c>
-      <c r="F8" s="40">
-        <v>236</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="41"/>
+      <c r="C8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="66"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1288,22 +1296,12 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="37">
-        <v>43921</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.59722222222222221</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.68055555555555547</v>
-      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="5">
-        <v>120</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>76</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1313,21 +1311,11 @@
         <v>4</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.83680555555555547</v>
-      </c>
-      <c r="E10" s="6">
-        <v>15</v>
-      </c>
-      <c r="F10" s="5">
-        <v>150</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>76</v>
-      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -1336,22 +1324,12 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7">
-        <v>43922</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.78472222222222221</v>
-      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="5">
-        <v>125</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="31"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1360,24 +1338,12 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7">
-        <v>43923</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.34722222222222227</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.41388888888888892</v>
-      </c>
-      <c r="E12" s="6">
-        <v>23</v>
-      </c>
-      <c r="F12" s="5">
-        <v>73</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -1387,19 +1353,11 @@
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.56944444444444442</v>
-      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="5">
-        <v>130</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -1409,19 +1367,11 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.80694444444444446</v>
-      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="5">
-        <v>142</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>80</v>
-      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1492,7 +1442,7 @@
       <c r="E19" s="45"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>1016</v>
+        <v>0</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1517,6 +1467,429 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="55">
+        <v>43870</v>
+      </c>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="62"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43865</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <v>30</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
+        <v>43865</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <v>30</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43866</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>48</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
+        <v>43866</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.89444444444444438</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <v>30</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>195</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <v>85</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.67986111111111114</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <v>89</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7">
+        <v>43868</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <v>90</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7">
+        <v>43869</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <v>160</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7">
+        <v>43870</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <v>230</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7">
+        <v>43870</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <v>25</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>1012</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -1899,10 +2272,419 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1E625-AEC1-4959-BE11-B43C72FD971D}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="106" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43920</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5">
+        <v>40</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="38">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.94861111111111107</v>
+      </c>
+      <c r="E8" s="39">
+        <v>20</v>
+      </c>
+      <c r="F8" s="40">
+        <v>236</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="37">
+        <v>43921</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>120</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="E10" s="6">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5">
+        <v>150</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43922</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>125</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43923</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="E12" s="6">
+        <v>23</v>
+      </c>
+      <c r="F12" s="5">
+        <v>73</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <v>130</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.80694444444444446</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <v>142</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7">
+        <v>43924</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <v>70</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7">
+        <v>43925</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <v>40</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>1126</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E40E1A-5312-4ABD-B40E-50820F71C983}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="126" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="94" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2259,7 +3041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EA6F01-A62E-4B54-89CC-1CA4694260FA}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2643,7 +3425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD152465-B78F-4330-B82E-1079DE07011D}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2958,7 +3740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D5B9A5-82EB-41D0-B31E-F472544F2A17}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -3311,7 +4093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACF002-C02F-4F6D-A9DF-5CDFC75330FF}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -3716,7 +4498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4BA9E6-34DD-4C1C-AEEF-5A72BA45E7B5}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -4101,7 +4883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8DD912-1C37-45A7-B4D1-E4B8ABC30324}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -4460,427 +5242,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
-  <dimension ref="A1:J19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="3.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="55">
-        <v>43870</v>
-      </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17">
-        <v>1</v>
-      </c>
-      <c r="B7" s="18">
-        <v>43865</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0.86875000000000002</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0.88611111111111107</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21">
-        <v>30</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="22"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="18">
-        <v>43865</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.90972222222222221</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5">
-        <v>30</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7">
-        <v>43866</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.81944444444444453</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5">
-        <v>48</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7">
-        <v>43866</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.89444444444444438</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5">
-        <v>30</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7">
-        <v>43867</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.46875</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5">
-        <v>195</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7">
-        <v>43867</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5">
-        <v>85</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7">
-        <v>43867</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.67986111111111114</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5">
-        <v>89</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>8</v>
-      </c>
-      <c r="B14" s="7">
-        <v>43868</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5">
-        <v>90</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
-        <v>9</v>
-      </c>
-      <c r="B15" s="7">
-        <v>43869</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="D15" s="32">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5">
-        <v>160</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7">
-        <v>43870</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0.38680555555555557</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0.54861111111111105</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5">
-        <v>230</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
-        <v>11</v>
-      </c>
-      <c r="B17" s="7">
-        <v>43870</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0.78819444444444453</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0.80555555555555547</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5">
-        <v>25</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="23">
-        <v>12</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="30">
-        <f>SUM(F7:F18)</f>
-        <v>1012</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A2:J3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:B6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
54. tehtud, testid ei lähe läbi sest andmebaasi pole
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9634437-9944-45EE-8CDE-17B98250E9E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AF84E0-B87B-4A01-9796-CA8795E13293}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,7 +295,7 @@
     <t>6-12aprill</t>
   </si>
   <si>
-    <t>10. kodutöö</t>
+    <t>10. kodutöö + andmebaasi errorid</t>
   </si>
 </sst>
 </file>
@@ -766,6 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -802,10 +803,13 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -823,19 +827,15 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,7 +1153,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1172,68 +1172,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="64"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="E8" s="39"/>
       <c r="F8" s="40"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="66"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1433,13 +1433,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>0</v>
@@ -1490,68 +1490,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43870</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="62"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1856,13 +1856,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1012</v>
@@ -1913,68 +1913,68 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43863</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="62"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2237,13 +2237,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>920</v>
@@ -2295,66 +2295,66 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -2647,13 +2647,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1126</v>
@@ -2704,68 +2704,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43905</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -3008,13 +3008,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>835</v>
@@ -3065,68 +3065,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43905</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -3392,13 +3392,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1478</v>
@@ -3449,68 +3449,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43905</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -3707,13 +3707,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>0</v>
@@ -3764,68 +3764,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43888</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -4060,13 +4060,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>723</v>
@@ -4117,68 +4117,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43888</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -4465,13 +4465,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>999</v>
@@ -4522,68 +4522,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43884</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -4850,13 +4850,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>912</v>
@@ -4907,68 +4907,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="64">
         <v>43877</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -5211,13 +5211,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>735</v>

</xml_diff>

<commit_message>
Units repo testid ja muudatused repo testides
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AF84E0-B87B-4A01-9796-CA8795E13293}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3812C2-2A55-4787-B9F9-65F12D5F8D12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="86">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>10. kodutöö + andmebaasi errorid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. kodutöö </t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1156,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1269,7 +1272,9 @@
       <c r="C7" s="8">
         <v>0.79513888888888884</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="8">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
       <c r="G7" s="6" t="s">
@@ -1283,11 +1288,17 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="38"/>
+      <c r="B8" s="7">
+        <v>43928</v>
+      </c>
+      <c r="C8" s="38">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="E8" s="39"/>
       <c r="F8" s="40"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H8" s="43"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>

</xml_diff>

<commit_message>
Kõik Pages klassid ja testid korras
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3812C2-2A55-4787-B9F9-65F12D5F8D12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900322E8-E0CA-49EC-84A6-116D4BA7BA1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="86">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1276,7 +1276,9 @@
         <v>0.90972222222222221</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>165</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>84</v>
       </c>
@@ -1294,8 +1296,15 @@
       <c r="C8" s="38">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
+      <c r="D8" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E8" s="39">
+        <v>30</v>
+      </c>
+      <c r="F8" s="40">
+        <v>145</v>
+      </c>
       <c r="G8" s="6" t="s">
         <v>85</v>
       </c>
@@ -1308,11 +1317,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="37"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.90277777777777779</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="5">
+        <v>100</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1321,12 +1338,20 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="7">
+        <v>43929</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -1336,7 +1361,9 @@
         <v>5</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8">
+        <v>0.79861111111111116</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
@@ -1453,7 +1480,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Errorid eemaldatud, vaja ainult testid veel korda teha
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C6A249-DAF4-46EE-8C69-83C3EE664799}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4810DE6B-B33F-4D48-8D86-DD86501CDFC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="89">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Töö timmimine ja ülevaatus</t>
+  </si>
+  <si>
+    <t>Testide errodi ja UnitsPageTests korda</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1165,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1392,9 +1395,13 @@
       <c r="C12" s="8">
         <v>0.38194444444444442</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>90</v>
+      </c>
       <c r="G12" s="8" t="s">
         <v>87</v>
       </c>
@@ -1411,7 +1418,9 @@
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -1496,7 +1505,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>640</v>
+        <v>730</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
2 viimast sisulist testiviga veel
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4810DE6B-B33F-4D48-8D86-DD86501CDFC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7552BFA3-F5F7-480E-9016-BE71127B00CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="510" windowWidth="19200" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 11" sheetId="13" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="91">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -307,7 +307,13 @@
     <t>Töö timmimine ja ülevaatus</t>
   </si>
   <si>
-    <t>Testide errodi ja UnitsPageTests korda</t>
+    <t>Testide errorid ja UnitsPageTests korda</t>
+  </si>
+  <si>
+    <t>PluralSight Scrum Fundamentals + konspekt</t>
+  </si>
+  <si>
+    <t>Testide veel korda</t>
   </si>
 </sst>
 </file>
@@ -1164,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BEF23C-5D4F-4A0C-A005-79341DDADDA7}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1357,7 +1363,9 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>135</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>85</v>
       </c>
@@ -1414,12 +1422,18 @@
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="6">
+        <v>75</v>
+      </c>
       <c r="G13" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1430,11 +1444,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.61111111111111105</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="5">
+        <v>65</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1444,11 +1466,15 @@
         <v>9</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+      <c r="C15" s="8">
+        <v>0.66319444444444442</v>
+      </c>
       <c r="D15" s="32"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -1505,7 +1531,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>730</v>
+        <v>1005</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
KÕIK ERRRORID KORRAS MOTHERFKING SHIT IS DONE
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7552BFA3-F5F7-480E-9016-BE71127B00CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138C6D38-E09B-4EB3-BD55-93611B209E07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="510" windowWidth="19200" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1469,9 +1469,13 @@
       <c r="C15" s="8">
         <v>0.66319444444444442</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="32">
+        <v>0.74305555555555547</v>
+      </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>115</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>90</v>
       </c>
@@ -1531,7 +1535,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>1005</v>
+        <v>1120</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>